<commit_message>
Changed some names Started working on OK PASS feature at both front and end added two properties to card added function in cardsController added service at dbService
</commit_message>
<xml_diff>
--- a/Frontend/input/example1card.xlsx
+++ b/Frontend/input/example1card.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Danni\source\repos\MemoryCards\test\MemoryCards\front-end\input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Danni\source\repos\MemoryCards\Frontend\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BAAA174-D535-4C66-92ED-9587054DF968}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7247767-7A84-45AE-A670-A5797C9A372C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11790" yWindow="7365" windowWidth="24585" windowHeight="13440" xr2:uid="{F9F7E55B-6084-438A-B6B0-D0D9AF79A29B}"/>
+    <workbookView xWindow="43065" yWindow="2940" windowWidth="23565" windowHeight="9180" xr2:uid="{F9F7E55B-6084-438A-B6B0-D0D9AF79A29B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -56,10 +56,10 @@
     <t>9+1</t>
   </si>
   <si>
-    <t>back</t>
-  </si>
-  <si>
-    <t>front</t>
+    <t>Question</t>
+  </si>
+  <si>
+    <t>Answer</t>
   </si>
 </sst>
 </file>
@@ -434,7 +434,7 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>